<commit_message>
[ProjRech] Envoi de la version 2B complète
</commit_message>
<xml_diff>
--- a/master2/output/trans_problème_schema.xlsx
+++ b/master2/output/trans_problème_schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\master2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\master2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D33D039-7433-4342-A6EC-3A4A5E00DB33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB58FB4D-F5FB-48AB-AEB9-4F6E1B1F0E7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5827,7 +5827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5858,6 +5858,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5871,7 +5877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5880,6 +5886,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22737,12 +22744,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F371"/>
+  <dimension ref="A1:F373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C370"/>
+      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F369" sqref="F369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22789,7 +22795,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>283</v>
       </c>
@@ -22820,7 +22826,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>283</v>
       </c>
@@ -22834,7 +22840,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>284</v>
       </c>
@@ -22848,13 +22854,16 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>284</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>303</v>
       </c>
@@ -22862,7 +22871,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>283</v>
       </c>
@@ -22876,7 +22885,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>289</v>
       </c>
@@ -22890,7 +22899,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>289</v>
       </c>
@@ -22904,7 +22913,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>287</v>
       </c>
@@ -22918,13 +22927,16 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>284</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
+      <c r="D12" s="8">
+        <v>2</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>313</v>
       </c>
@@ -22932,7 +22944,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>283</v>
       </c>
@@ -22963,7 +22975,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>283</v>
       </c>
@@ -23081,7 +23093,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>283</v>
       </c>
@@ -23095,7 +23107,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>287</v>
       </c>
@@ -23109,13 +23121,16 @@
         <v>336</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>284</v>
       </c>
       <c r="C24" t="s">
         <v>68</v>
       </c>
+      <c r="D24" s="8">
+        <v>2</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>337</v>
       </c>
@@ -23123,7 +23138,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>283</v>
       </c>
@@ -23137,7 +23152,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>287</v>
       </c>
@@ -23151,7 +23166,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>283</v>
       </c>
@@ -23165,7 +23180,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>283</v>
       </c>
@@ -23179,7 +23194,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>283</v>
       </c>
@@ -23210,7 +23225,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>283</v>
       </c>
@@ -23275,7 +23290,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>283</v>
       </c>
@@ -23324,7 +23339,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>285</v>
       </c>
@@ -23373,7 +23388,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>283</v>
       </c>
@@ -23404,7 +23419,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>283</v>
       </c>
@@ -23418,7 +23433,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>285</v>
       </c>
@@ -23449,7 +23464,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>283</v>
       </c>
@@ -23480,7 +23495,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>285</v>
       </c>
@@ -23494,7 +23509,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>285</v>
       </c>
@@ -23508,13 +23523,16 @@
         <v>388</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>284</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
+      <c r="D50" s="8">
+        <v>2</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>389</v>
       </c>
@@ -23522,13 +23540,16 @@
         <v>390</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>284</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
       </c>
+      <c r="D51" s="8">
+        <v>2</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>391</v>
       </c>
@@ -23536,7 +23557,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>283</v>
       </c>
@@ -23550,7 +23571,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -23582,7 +23603,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>283</v>
       </c>
@@ -23596,7 +23617,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>287</v>
       </c>
@@ -23645,7 +23666,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>283</v>
       </c>
@@ -23693,7 +23714,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>284</v>
       </c>
@@ -23724,7 +23745,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>283</v>
       </c>
@@ -23738,7 +23759,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>284</v>
       </c>
@@ -23752,7 +23773,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>285</v>
       </c>
@@ -23784,13 +23805,16 @@
         <v>424</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>284</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
+      <c r="D68" s="8">
+        <v>2</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>425</v>
       </c>
@@ -23798,7 +23822,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>283</v>
       </c>
@@ -23829,7 +23853,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>283</v>
       </c>
@@ -23843,7 +23867,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>283</v>
       </c>
@@ -23857,7 +23881,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>283</v>
       </c>
@@ -23888,7 +23912,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>283</v>
       </c>
@@ -23902,7 +23926,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>288</v>
       </c>
@@ -23916,7 +23940,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>283</v>
       </c>
@@ -23930,7 +23954,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>283</v>
       </c>
@@ -23978,7 +24002,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>283</v>
       </c>
@@ -23992,7 +24016,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>283</v>
       </c>
@@ -24006,7 +24030,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>283</v>
       </c>
@@ -24020,7 +24044,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>283</v>
       </c>
@@ -24034,7 +24058,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>283</v>
       </c>
@@ -24065,7 +24089,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>283</v>
       </c>
@@ -24079,7 +24103,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>284</v>
       </c>
@@ -24093,7 +24117,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>283</v>
       </c>
@@ -24124,7 +24148,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>283</v>
       </c>
@@ -24138,7 +24162,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>288</v>
       </c>
@@ -24152,7 +24176,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>290</v>
       </c>
@@ -24166,12 +24190,15 @@
         <v>476</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>284</v>
       </c>
       <c r="C94" t="s">
         <v>31</v>
+      </c>
+      <c r="D94" s="8">
+        <v>2</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>477</v>
@@ -24232,7 +24259,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>285</v>
       </c>
@@ -24246,7 +24273,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>288</v>
       </c>
@@ -24260,12 +24287,15 @@
         <v>488</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>284</v>
       </c>
       <c r="C100" t="s">
         <v>11</v>
+      </c>
+      <c r="D100" s="8">
+        <v>2</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>489</v>
@@ -24291,7 +24321,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>283</v>
       </c>
@@ -24340,7 +24370,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>283</v>
       </c>
@@ -24354,13 +24384,16 @@
         <v>500</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>284</v>
       </c>
       <c r="C106" t="s">
         <v>121</v>
       </c>
+      <c r="D106" s="8">
+        <v>2</v>
+      </c>
       <c r="E106" s="1" t="s">
         <v>501</v>
       </c>
@@ -24368,7 +24401,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>285</v>
       </c>
@@ -24382,7 +24415,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>283</v>
       </c>
@@ -24396,7 +24429,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>290</v>
       </c>
@@ -24427,7 +24460,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>284</v>
       </c>
@@ -24475,7 +24508,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>283</v>
       </c>
@@ -24489,7 +24522,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>283</v>
       </c>
@@ -24503,7 +24536,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>283</v>
       </c>
@@ -24517,7 +24550,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>283</v>
       </c>
@@ -24567,7 +24600,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>287</v>
       </c>
@@ -24581,7 +24614,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>283</v>
       </c>
@@ -24595,7 +24628,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>283</v>
       </c>
@@ -24609,7 +24642,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>285</v>
       </c>
@@ -24623,7 +24656,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>283</v>
       </c>
@@ -24637,7 +24670,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>283</v>
       </c>
@@ -24651,7 +24684,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>283</v>
       </c>
@@ -24665,7 +24698,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>283</v>
       </c>
@@ -24696,7 +24729,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>283</v>
       </c>
@@ -24710,7 +24743,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>283</v>
       </c>
@@ -24724,7 +24757,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>283</v>
       </c>
@@ -24738,7 +24771,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>285</v>
       </c>
@@ -24752,7 +24785,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>283</v>
       </c>
@@ -24766,7 +24799,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>285</v>
       </c>
@@ -24780,7 +24813,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>287</v>
       </c>
@@ -24794,7 +24827,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>283</v>
       </c>
@@ -24808,7 +24841,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>285</v>
       </c>
@@ -24822,7 +24855,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>283</v>
       </c>
@@ -24836,7 +24869,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>283</v>
       </c>
@@ -24867,7 +24900,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>283</v>
       </c>
@@ -24881,7 +24914,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>283</v>
       </c>
@@ -24895,7 +24928,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>283</v>
       </c>
@@ -24926,7 +24959,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>283</v>
       </c>
@@ -24975,7 +25008,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>284</v>
       </c>
@@ -24989,7 +25022,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>283</v>
       </c>
@@ -25003,7 +25036,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>283</v>
       </c>
@@ -25017,7 +25050,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>288</v>
       </c>
@@ -25031,12 +25064,15 @@
         <v>592</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>284</v>
       </c>
       <c r="C152" t="s">
         <v>152</v>
+      </c>
+      <c r="D152" s="8">
+        <v>2</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>593</v>
@@ -25062,7 +25098,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>283</v>
       </c>
@@ -25076,7 +25112,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>285</v>
       </c>
@@ -25107,7 +25143,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>286</v>
       </c>
@@ -25121,7 +25157,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>283</v>
       </c>
@@ -25135,7 +25171,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>283</v>
       </c>
@@ -25149,7 +25185,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>283</v>
       </c>
@@ -25163,7 +25199,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>283</v>
       </c>
@@ -25194,7 +25230,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>283</v>
       </c>
@@ -25243,7 +25279,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>285</v>
       </c>
@@ -25257,7 +25293,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>283</v>
       </c>
@@ -25305,7 +25341,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>283</v>
       </c>
@@ -25319,7 +25355,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>283</v>
       </c>
@@ -25333,7 +25369,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>283</v>
       </c>
@@ -25347,7 +25383,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>286</v>
       </c>
@@ -25361,7 +25397,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>285</v>
       </c>
@@ -25392,7 +25428,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>287</v>
       </c>
@@ -25406,7 +25442,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>283</v>
       </c>
@@ -25437,7 +25473,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>285</v>
       </c>
@@ -25469,7 +25505,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>283</v>
       </c>
@@ -25483,7 +25519,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>285</v>
       </c>
@@ -25497,7 +25533,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>283</v>
       </c>
@@ -25528,7 +25564,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>286</v>
       </c>
@@ -25542,7 +25578,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>283</v>
       </c>
@@ -25573,7 +25609,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>283</v>
       </c>
@@ -25587,7 +25623,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>283</v>
       </c>
@@ -25601,7 +25637,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>283</v>
       </c>
@@ -25615,7 +25651,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>283</v>
       </c>
@@ -25646,7 +25682,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>283</v>
       </c>
@@ -25660,7 +25696,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>283</v>
       </c>
@@ -25674,7 +25710,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>283</v>
       </c>
@@ -25723,7 +25759,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>283</v>
       </c>
@@ -25737,7 +25773,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>286</v>
       </c>
@@ -25751,7 +25787,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>283</v>
       </c>
@@ -25782,7 +25818,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>283</v>
       </c>
@@ -25796,7 +25832,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>283</v>
       </c>
@@ -25827,12 +25863,15 @@
         <v>698</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>284</v>
       </c>
       <c r="C205" t="s">
         <v>182</v>
+      </c>
+      <c r="D205" s="8">
+        <v>2</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>699</v>
@@ -25859,7 +25898,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>283</v>
       </c>
@@ -25873,7 +25912,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>283</v>
       </c>
@@ -25904,7 +25943,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>285</v>
       </c>
@@ -25918,7 +25957,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>283</v>
       </c>
@@ -25932,7 +25971,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>283</v>
       </c>
@@ -25946,7 +25985,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>283</v>
       </c>
@@ -25960,7 +25999,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>283</v>
       </c>
@@ -25974,7 +26013,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>283</v>
       </c>
@@ -25988,7 +26027,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>283</v>
       </c>
@@ -26002,7 +26041,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>285</v>
       </c>
@@ -26033,7 +26072,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>285</v>
       </c>
@@ -26064,7 +26103,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>283</v>
       </c>
@@ -26095,7 +26134,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>285</v>
       </c>
@@ -26109,12 +26148,15 @@
         <v>736</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>284</v>
       </c>
       <c r="C224" t="s">
         <v>14</v>
+      </c>
+      <c r="D224" s="8">
+        <v>2</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>737</v>
@@ -26158,7 +26200,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>283</v>
       </c>
@@ -26175,7 +26217,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>283</v>
       </c>
@@ -26189,7 +26231,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>283</v>
       </c>
@@ -26203,7 +26245,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>283</v>
       </c>
@@ -26217,7 +26259,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>283</v>
       </c>
@@ -26231,7 +26273,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>283</v>
       </c>
@@ -26262,7 +26304,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>286</v>
       </c>
@@ -26293,7 +26335,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>283</v>
       </c>
@@ -26307,7 +26349,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>283</v>
       </c>
@@ -26321,7 +26363,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>283</v>
       </c>
@@ -26369,7 +26411,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>285</v>
       </c>
@@ -26383,7 +26425,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>283</v>
       </c>
@@ -26397,7 +26439,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>284</v>
       </c>
@@ -26411,7 +26453,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>283</v>
       </c>
@@ -26459,7 +26501,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>283</v>
       </c>
@@ -26490,7 +26532,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>289</v>
       </c>
@@ -26504,7 +26546,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>283</v>
       </c>
@@ -26535,7 +26577,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>285</v>
       </c>
@@ -26566,12 +26608,15 @@
         <v>796</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>284</v>
       </c>
       <c r="C254" t="s">
         <v>49</v>
+      </c>
+      <c r="D254" s="8">
+        <v>2</v>
       </c>
       <c r="E254" s="1" t="s">
         <v>797</v>
@@ -26651,7 +26696,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>285</v>
       </c>
@@ -26665,7 +26710,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>283</v>
       </c>
@@ -26679,7 +26724,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>283</v>
       </c>
@@ -26693,7 +26738,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>286</v>
       </c>
@@ -26724,7 +26769,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>283</v>
       </c>
@@ -26738,7 +26783,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>286</v>
       </c>
@@ -26752,7 +26797,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>285</v>
       </c>
@@ -26766,7 +26811,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>283</v>
       </c>
@@ -26780,7 +26825,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>283</v>
       </c>
@@ -26811,12 +26856,15 @@
         <v>828</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>284</v>
       </c>
       <c r="C270" t="s">
         <v>226</v>
+      </c>
+      <c r="D270" s="8">
+        <v>2</v>
       </c>
       <c r="E270" s="1" t="s">
         <v>829</v>
@@ -26842,7 +26890,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>288</v>
       </c>
@@ -26856,7 +26904,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>283</v>
       </c>
@@ -26870,7 +26918,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>286</v>
       </c>
@@ -26972,7 +27020,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>287</v>
       </c>
@@ -26986,7 +27034,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>286</v>
       </c>
@@ -27017,7 +27065,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>287</v>
       </c>
@@ -27031,7 +27079,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -27045,7 +27093,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>283</v>
       </c>
@@ -27093,7 +27141,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>283</v>
       </c>
@@ -27161,7 +27209,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>283</v>
       </c>
@@ -27175,7 +27223,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>283</v>
       </c>
@@ -27189,7 +27237,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>288</v>
       </c>
@@ -27203,7 +27251,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>283</v>
       </c>
@@ -27234,7 +27282,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>283</v>
       </c>
@@ -27248,7 +27296,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>283</v>
       </c>
@@ -27262,7 +27310,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>283</v>
       </c>
@@ -27276,7 +27324,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>283</v>
       </c>
@@ -27341,7 +27389,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>283</v>
       </c>
@@ -27355,7 +27403,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>283</v>
       </c>
@@ -27389,7 +27437,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>286</v>
       </c>
@@ -27403,7 +27451,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>283</v>
       </c>
@@ -27434,7 +27482,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>283</v>
       </c>
@@ -27448,7 +27496,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>283</v>
       </c>
@@ -27530,7 +27578,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>286</v>
       </c>
@@ -27561,7 +27609,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>283</v>
       </c>
@@ -27643,7 +27691,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>285</v>
       </c>
@@ -27657,7 +27705,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>283</v>
       </c>
@@ -27671,7 +27719,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>291</v>
       </c>
@@ -27702,7 +27750,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>283</v>
       </c>
@@ -27716,13 +27764,16 @@
         <v>944</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>284</v>
       </c>
       <c r="C328" t="s">
         <v>36</v>
       </c>
+      <c r="D328" s="8">
+        <v>2</v>
+      </c>
       <c r="E328" s="1" t="s">
         <v>945</v>
       </c>
@@ -27730,7 +27781,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>283</v>
       </c>
@@ -27744,7 +27795,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>283</v>
       </c>
@@ -27775,7 +27826,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>292</v>
       </c>
@@ -27789,7 +27840,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>283</v>
       </c>
@@ -27820,7 +27871,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>286</v>
       </c>
@@ -27834,7 +27885,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>283</v>
       </c>
@@ -27848,7 +27899,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>287</v>
       </c>
@@ -27862,7 +27913,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>283</v>
       </c>
@@ -27876,7 +27927,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>291</v>
       </c>
@@ -27924,7 +27975,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>286</v>
       </c>
@@ -28006,7 +28057,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>283</v>
       </c>
@@ -28020,7 +28071,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>283</v>
       </c>
@@ -28105,12 +28156,15 @@
         <v>994</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>284</v>
       </c>
       <c r="C353" t="s">
         <v>269</v>
+      </c>
+      <c r="D353" s="8">
+        <v>2</v>
       </c>
       <c r="E353" s="1" t="s">
         <v>995</v>
@@ -28190,7 +28244,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>283</v>
       </c>
@@ -28204,7 +28258,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>283</v>
       </c>
@@ -28235,7 +28289,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>283</v>
       </c>
@@ -28249,7 +28303,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>283</v>
       </c>
@@ -28263,7 +28317,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>283</v>
       </c>
@@ -28277,7 +28331,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>283</v>
       </c>
@@ -28291,7 +28345,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>284</v>
       </c>
@@ -28305,7 +28359,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>283</v>
       </c>
@@ -28319,7 +28373,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>288</v>
       </c>
@@ -28350,12 +28404,15 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>284</v>
       </c>
       <c r="C369" t="s">
         <v>281</v>
+      </c>
+      <c r="D369" s="8">
+        <v>2</v>
       </c>
       <c r="E369" s="1" t="s">
         <v>1027</v>
@@ -28381,7 +28438,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>283</v>
       </c>
@@ -28395,14 +28452,14 @@
         <v>1032</v>
       </c>
     </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D373">
+        <f>COUNTIF(D1:D371, 2)</f>
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C371" xr:uid="{60317446-7AB8-411F-95B5-BAE095E66695}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C371" xr:uid="{60317446-7AB8-411F-95B5-BAE095E66695}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>